<commit_message>
EML.XML content moved to Excel.
</commit_message>
<xml_diff>
--- a/test_data/resources/dwca_matrix_zoobenthos_nat.xlsx
+++ b/test_data/resources/dwca_matrix_zoobenthos_nat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="687" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="687" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dwc_columns" sheetId="12" r:id="rId1"/>
@@ -1873,7 +1873,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>182</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>182</v>
       </c>
@@ -1901,10 +1901,10 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
@@ -3092,7 +3092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -3300,14 +3300,14 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="6" max="6" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3379,7 +3379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>

</xml_diff>